<commit_message>
Changed title of GUI
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Willi\Desktop\GuiPractice\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Willi\Desktop\Presentation1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9C34BD0C-3986-4FC3-BF8D-CDA50387EB8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{77612055-55AD-4099-8541-CEF2E208F6F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4673" yWindow="1605" windowWidth="14400" windowHeight="7373" xr2:uid="{C3C5F6DA-BEBC-4562-9769-A6F77967645A}"/>
+    <workbookView xWindow="4673" yWindow="1605" windowWidth="14400" windowHeight="7373" xr2:uid="{93FAC6E7-3A2C-4333-A70A-23BA4AB0A973}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -381,7 +381,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{027AB7D7-1C92-4478-BB7D-4E1C7258BA29}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A530D247-197D-4C45-B6D9-ACD13EE6926B}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Added xlwings and docx functions
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Willi\Desktop\Presentation1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{77612055-55AD-4099-8541-CEF2E208F6F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C800417F-D881-43C7-AB2B-0E8BBA8DC434}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4673" yWindow="1605" windowWidth="14400" windowHeight="7373" xr2:uid="{93FAC6E7-3A2C-4333-A70A-23BA4AB0A973}"/>
+    <workbookView xWindow="4673" yWindow="1605" windowWidth="14400" windowHeight="7373" xr2:uid="{FB6F84C1-A8CD-42C7-B97F-F488D54664E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -381,7 +381,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A530D247-197D-4C45-B6D9-ACD13EE6926B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{785FCCA1-E0D5-4387-A58C-A76E6A0D9335}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Added xlwings and docx functions and edited text
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Willi\Desktop\Presentation1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C800417F-D881-43C7-AB2B-0E8BBA8DC434}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7AD16603-03AD-4022-8270-8250930C6A08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4673" yWindow="1605" windowWidth="14400" windowHeight="7373" xr2:uid="{FB6F84C1-A8CD-42C7-B97F-F488D54664E6}"/>
+    <workbookView xWindow="368" yWindow="368" windowWidth="14399" windowHeight="7372" xr2:uid="{A994F93F-D36C-4C08-9155-C486B048CC03}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -381,7 +381,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{785FCCA1-E0D5-4387-A58C-A76E6A0D9335}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71997E18-40B8-40DF-8F1D-786C9313DCCC}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
small changes to strings
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Willi\Desktop\Presentation1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7AD16603-03AD-4022-8270-8250930C6A08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A3535D9A-6413-4706-A532-3726DEC1B014}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="368" yWindow="368" windowWidth="14399" windowHeight="7372" xr2:uid="{A994F93F-D36C-4C08-9155-C486B048CC03}"/>
+    <workbookView xWindow="2543" yWindow="2543" windowWidth="14400" windowHeight="7372" xr2:uid="{5578FAD6-0FAE-4A1C-9D79-7A31C1F427D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -381,7 +381,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71997E18-40B8-40DF-8F1D-786C9313DCCC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE130FD5-ABFF-47A6-8296-819BB2389CFA}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>